<commit_message>
Added updated tools translation
</commit_message>
<xml_diff>
--- a/webcentral/doc/01_data/02_tool_over/tools_with_weatherdata.xlsx
+++ b/webcentral/doc/01_data/02_tool_over/tools_with_weatherdata.xlsx
@@ -8,8 +8,8 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="German" sheetId="1" state="visible" r:id="rId3"/>
-    <sheet name="English" sheetId="2" state="visible" r:id="rId4"/>
+    <sheet name="German" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="English" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4763" uniqueCount="1369">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4763" uniqueCount="1375">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -3290,7 +3290,7 @@
     <t xml:space="preserve">Chargeable;;Open-Source</t>
   </si>
   <si>
-    <t xml:space="preserve">MongoDB is mainly distributed under an open source license. However, it also offers a commercial version with additional functions and support (for details, see https://www.mongodb.com/pricing)</t>
+    <t xml:space="preserve">MongoDB is mainly distributed under an open-source license. However, it also offers a commercial version with additional functions and support (for details, see https://www.mongodb.com/pricing)</t>
   </si>
   <si>
     <t xml:space="preserve">C# is a type-safe object-oriented general-purpose programming language.</t>
@@ -3404,7 +3404,7 @@
     <t xml:space="preserve">command line</t>
   </si>
   <si>
-    <t xml:space="preserve">a Modelica library</t>
+    <t xml:space="preserve">A Modelica library</t>
   </si>
   <si>
     <t xml:space="preserve">License details: https://github.com/RWTH-EBC/BESMod/blob/main/LICENSE</t>
@@ -3419,6 +3419,9 @@
     <t xml:space="preserve">Monitoring;;Optimization;;Planning</t>
   </si>
   <si>
+    <t xml:space="preserve">pl</t>
+  </si>
+  <si>
     <t xml:space="preserve">Julia is a highly developed, powerful dynamic programming language for technical calculations. It is designed for numerical and scientific calculations.</t>
   </si>
   <si>
@@ -3476,7 +3479,7 @@
     <t xml:space="preserve">Building;;Quarters/Networks</t>
   </si>
   <si>
-    <t xml:space="preserve">OpenModelica is a free open source environment based on the Modelica modeling language for modeling, simulating, optimizing and analyzing complex dynamic systems.</t>
+    <t xml:space="preserve">OpenModelica is a free open-source environment based on the Modelica modeling language for modeling, simulating, optimizing and analyzing complex dynamic systems.</t>
   </si>
   <si>
     <t xml:space="preserve">Microsoft Visio is a visualization program from Microsoft for Windows.</t>
@@ -3494,7 +3497,7 @@
     <t xml:space="preserve">End users;;Computer scientists/software developers;;Engineers</t>
   </si>
   <si>
-    <t xml:space="preserve">The PostgreSQL License is a liberal open source license that is similar to the BSD or MIT license.</t>
+    <t xml:space="preserve">The PostgreSQL License is a liberal open-source license that is similar to the BSD or MIT license.</t>
   </si>
   <si>
     <t xml:space="preserve">R is a free software environment for statistical calculations and graphics.</t>
@@ -3512,7 +3515,7 @@
     <t xml:space="preserve">operational</t>
   </si>
   <si>
-    <t xml:space="preserve">IfcOpenShell is an open source software library, available in C++ and Python, designed to facilitate work with the Industry Foundation Classes (IFC) file format. The IFC file format can be used to describe building and construction data and is commonly used for Building Information Modeling.</t>
+    <t xml:space="preserve">IfcOpenShell is an open-source software library, available in C++ and Python, designed to facilitate work with the Industry Foundation Classes (IFC) file format. The IFC file format can be used to describe building and construction data and is commonly used for Building Information Modeling.</t>
   </si>
   <si>
     <t xml:space="preserve">Planning;;Simulation;;Visualization</t>
@@ -3524,7 +3527,7 @@
     <t xml:space="preserve">Graphical user interface;;Web-based user interface</t>
   </si>
   <si>
-    <t xml:space="preserve">GitLab is mainly distributed under an open source license. However, GitLab also offers a commercial version with additional functions and support (for details, see https://about.gitlab.com/pricing/).</t>
+    <t xml:space="preserve">GitLab is mainly distributed under an open-source license. However, GitLab also offers a commercial version with additional functions and support (for details, see https://about.gitlab.com/pricing/).</t>
   </si>
   <si>
     <t xml:space="preserve">SolidWorks develops and markets software for computer-aided design, computer-aided engineering, 3D CAD design and collaboration, analysis and product data management. SolidWorks is used to create parametric models, assemblies and technical drawings.</t>
@@ -3539,6 +3542,9 @@
     <t xml:space="preserve">Licensing details: https://www.sqlite.org/copyright.html</t>
   </si>
   <si>
+    <t xml:space="preserve">DELPHIN</t>
+  </si>
+  <si>
     <t xml:space="preserve">DELPHIN is a simulation software for coupled heat, moisture, air and salt transport in porous building materials.</t>
   </si>
   <si>
@@ -3566,10 +3572,10 @@
     <t xml:space="preserve">uesgraphs is a Python library for describing urban energy systems and managing their data in a Python graph structure. The graph class in networkx has been extended to represent buildings and energy networks in the graph. uesgraphs can be used as a basis for analyzing energy network structures, evaluating district heating systems or creating simulation models.</t>
   </si>
   <si>
-    <t xml:space="preserve">a Python library</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The EPN initially supports companies in positioning themselves in a digital ecosystem. In addition, the tool offers assistance in identifying suitable business model patterns that can ultimately be combined to form a specific business model.</t>
+    <t xml:space="preserve">A Python library</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The EPN initially supports companies in positioning themselves in a digital ecosystem. In addition, the tool provides assistance in identifying suitable business model patterns that can ultimately be combined to form a specific business model.</t>
   </si>
   <si>
     <t xml:space="preserve">SIR 3S is a software tool developed for the calculation, simulation, analysis and optimization of flow processes in gas, water and heat supply networks as well as other piping systems.</t>
@@ -3578,7 +3584,7 @@
     <t xml:space="preserve">Quarters/Networks;;Region/Country</t>
   </si>
   <si>
-    <t xml:space="preserve">ENTIGRIS is an electricity market model for analyzing energy systems from an economic perspective. It takes into account various factors, including actor constellations and economic indicators, to provide insights into the development of energy systems.</t>
+    <t xml:space="preserve">ENTIGRIS is an electricity market model for analyzing energy systems from an economic perspective. It considers various factors, including actor constellations and economic indicators, to provide insights into the development of energy systems.</t>
   </si>
   <si>
     <t xml:space="preserve">Region/Country</t>
@@ -3587,7 +3593,7 @@
     <t xml:space="preserve">Unknown</t>
   </si>
   <si>
-    <t xml:space="preserve">Eclipse Mosquitto is an open source (EPL/EDL licensed) message broker that works with the MQTT protocol</t>
+    <t xml:space="preserve">Eclipse Mosquitto is an open-source (EPL/EDL licensed) message broker that works with the MQTT protocol</t>
   </si>
   <si>
     <t xml:space="preserve">Monitoring;;Advanced Control;;Control</t>
@@ -3665,10 +3671,7 @@
     <t xml:space="preserve">before 2012</t>
   </si>
   <si>
-    <t xml:space="preserve">TEASER (Tool for Energy Analysis and Simulation for Efficient Retrofit) is an open tool for urban energy modeling of the existing building stock. TEASER offers a user-friendly interface for different data sources (e.g. CityGML, SQL, ...) as well as the possibility for data enrichment if required. In addition, TEASER enables the export of ready-to-use Modelica simulation models for all libraries that support the Modelica IBPSA library.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">a Python Library</t>
+    <t xml:space="preserve">TEASER (Tool for Energy Analysis and Simulation for Efficient Retrofit) is an open tool for urban energy modeling of the existing building stock. TEASER offers a user-friendly interface for different data sources (e.g., CityGML, SQL, ...) as well as the possibility for data enrichment if required. In addition, TEASER enables the export of ready-to-use Modelica simulation models for all libraries that support the Modelica IBPSA library.</t>
   </si>
   <si>
     <t xml:space="preserve">The AI Navigator uses examples to show which tasks artificial intelligence can take on in service development and service management. Typical activities are listed for each phase of the service life cycle, for which AI solutions available on the market and practical examples are provided where available.</t>
@@ -3689,6 +3692,9 @@
     <t xml:space="preserve">Building</t>
   </si>
   <si>
+    <t xml:space="preserve">Wind Heating 2.0 Planning Tool</t>
+  </si>
+  <si>
     <t xml:space="preserve">Wind Heating 2.0 Planning Tool is a software for planning and optimizing Wind Heating 2.0 buildings that use surplus wind energy for heating.</t>
   </si>
   <si>
@@ -3827,7 +3833,10 @@
     <t xml:space="preserve">Monitoring;;Visualization</t>
   </si>
   <si>
-    <t xml:space="preserve">The district generator is a web tool for comparing supply concepts for districts. It contains a load profile generator for customizable building stock in districts, design optimization of central supply systems, operational optimization of various technology scenarios and evaluation based on KPIs.</t>
+    <t xml:space="preserve">District generator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">District generator is a web tool for comparing supply concepts for districts. It contains a load profile generator for customizable building stock in districts, design optimization of central supply systems, operational optimization of various technology scenarios and evaluation based on KPIs.</t>
   </si>
   <si>
     <t xml:space="preserve">Research/Teaching;;Administration</t>
@@ -3866,6 +3875,9 @@
     <t xml:space="preserve">EED is a PC program for designing vertical borehole heat exchangers</t>
   </si>
   <si>
+    <t xml:space="preserve">RKW Digitialization-Cockpit</t>
+  </si>
+  <si>
     <t xml:space="preserve">The Cockpit is intended to provide initial guidance on the topic of digitalization in companies. It consists of a constantly growing collection of company examples from various sectors with concrete points of reference and food for thought for a digitalization strategy.</t>
   </si>
   <si>
@@ -3887,7 +3899,7 @@
     <t xml:space="preserve">IDA Indoor Climate and Energy (IDA-ICE) is a software for simulating building performance</t>
   </si>
   <si>
-    <t xml:space="preserve">EHDO (Energy hub design optimization) is a web tool to support the planning process of complex energy supply systems. EHDO supports the planning of future energy supply systems and the assessment of the potential of renewable energies and future energy sources such as hydrogen. A wide range of innovative technologies such as fuel cells, electrolyzers, hydrogen storage, photovoltaic and wind power plants as well as biomass and waste-to-energy technologies can be taken into account in the tool.</t>
+    <t xml:space="preserve">EHDO (Energy hub design optimization) is a web tool to support the planning process of complex energy supply systems. EHDO supports the planning of future energy supply systems and the assessment of the potential of renewable energies and future energy sources such as hydrogen. A wide range of innovative technologies such as fuel cells, electrolyzers, hydrogen storage, photovoltaic and wind power plants as well as biomass and waste-to-energy technologies can be considered in the tool.</t>
   </si>
   <si>
     <t xml:space="preserve">Python is a universal, commonly interpreted, high-level programming language.</t>
@@ -3899,7 +3911,7 @@
     <t xml:space="preserve">Plotly.js is a library for JavaScript applications that use graphs and charts. It is a data visualization library built on top of D3 JS and Stack dot GL.</t>
   </si>
   <si>
-    <t xml:space="preserve">a Javascript library</t>
+    <t xml:space="preserve">A Javascript library</t>
   </si>
   <si>
     <t xml:space="preserve">For details see https://github.com/plotly/plotly.js?tab=License-1-ov-file</t>
@@ -3911,10 +3923,10 @@
     <t xml:space="preserve">Rhinoceros 3D is a software for computer-aided 3D modeling and computer-aided design, the full version can be tested for 90 days. After 90 days, saving and plug-ins will no longer work unless a license key is purchased. A student version is also available.</t>
   </si>
   <si>
-    <t xml:space="preserve">TimescaleDB is an open source SQL database for time series that extends PostgresSQL and is optimized for fast collections and complex queries.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TimescaleDB is an open source SQL database for time series that extends PostgresSQL and is optimized for fast collections and complex queries.for details see https://github.com/timescale/timescaledb/blob/main/LICENSE</t>
+    <t xml:space="preserve">TimescaleDB is an open-source SQL database for time series that extends PostgresSQL and is optimized for fast collections and complex queries.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TimescaleDB is an open-source SQL database for time series that extends PostgresSQL and is optimized for fast collections and complex queries. For details see https://github.com/timescale/timescaledb/blob/main/LICENSE</t>
   </si>
   <si>
     <t xml:space="preserve">COMSOL Multiphysics is a software for the simulation of physical processes that can be described by means of differential equations.</t>
@@ -3944,7 +3956,7 @@
     <t xml:space="preserve">EnergyPlus is a building energy simulation program for engineers and architects to model and simulate energy consumption for heating, cooling, ventilation, lighting as well as plug-and-process loads and water consumption in buildings.</t>
   </si>
   <si>
-    <t xml:space="preserve">InfluxDB is an open source database management system, especially for time series.</t>
+    <t xml:space="preserve">InfluxDB is an open-source database management system, especially for time series.</t>
   </si>
   <si>
     <t xml:space="preserve">Free version available, paid versions for professional applications</t>
@@ -3956,7 +3968,7 @@
     <t xml:space="preserve">LS-DYNA emerged from the 3D FEA program DYNA3D developed in 1976.</t>
   </si>
   <si>
-    <t xml:space="preserve">pandapipes is an easy-to-use network calculation program designed to automate the analysis of district heating and gas systems. It uses the pandas data analysis library and is also closely related to the pandapower power grid calculation program.</t>
+    <t xml:space="preserve">pandapipes is an easy-to-use network calculation program designed to automate the analysis of district heating and gas systems. It uses the panda data analysis library and is also closely related to the pandapower power grid calculation program.</t>
   </si>
   <si>
     <t xml:space="preserve">License details: https://pandapipes.readthedocs.io/en/latest/about/license.html</t>
@@ -3977,7 +3989,7 @@
     <t xml:space="preserve">MySQL is an open-source relational database management system that stores structured data in tables and is queried and managed using SQL.</t>
   </si>
   <si>
-    <t xml:space="preserve">CasADi is an open source software tool for numerical optimization in general and optimal control (i.e. optimization with differential equations) in particular.</t>
+    <t xml:space="preserve">CasADi is an open-source software tool for numerical optimization in general and optimal control (i.e. optimization with differential equations) in particular.</t>
   </si>
   <si>
     <t xml:space="preserve">Optimization;;Planning;;Advanced Control;;Control</t>
@@ -4013,7 +4025,7 @@
     <t xml:space="preserve">operational;;legal;;technical</t>
   </si>
   <si>
-    <t xml:space="preserve">Grafana is a cross-platform open source application for the graphical representation of data from various data sources such as InfluxDB, MySQL, PostgreSQL, Prometheus and Graphite. The captured raw data can then be output in various display formats.</t>
+    <t xml:space="preserve">Grafana is a cross-platform open-source application for the graphical representation of data from various data sources such as InfluxDB, MySQL, PostgreSQL, Prometheus and Graphite. The captured raw data can then be output in various display formats.</t>
   </si>
   <si>
     <t xml:space="preserve">Graphical user interface (plug-in for Excel)</t>
@@ -4025,7 +4037,7 @@
     <t xml:space="preserve">QGIS is a free geographic information system software for viewing, editing, capturing and analyzing spatial data.</t>
   </si>
   <si>
-    <t xml:space="preserve">OpenGeoSys (OGS) is a scientific open source project for the development of numerical methods for the simulation of thermo-hydro-mechanical-chemical (THMC) processes in porous and fractured media.</t>
+    <t xml:space="preserve">OpenGeoSys (OGS) is a scientific open-source project for the development of numerical methods for the simulation of thermo-hydro-mechanical-chemical (THMC) processes in porous and fractured media.</t>
   </si>
   <si>
     <t xml:space="preserve">CO2Calc4Quartier is a tool that was developed for evaluating district heating concepts with a particular focus on CO2 emissions.</t>
@@ -4055,16 +4067,19 @@
     <t xml:space="preserve">Optimization</t>
   </si>
   <si>
-    <t xml:space="preserve">The toolbox "Business model development in SMEs" contains a collection of tools that can enrich a business model development process. Each tool comes with instructions in PDF format and a Word template for customizing and printing.</t>
+    <t xml:space="preserve">Toolbox – “Business model development in SMEs”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The toolbox “Business model development in SMEs” contains a collection of tools that can enrich a business model development process. Each tool comes with instructions in PDF format and a Word template for customizing and printing.</t>
   </si>
   <si>
     <t xml:space="preserve">The ANSYS Fluids product family for fluid mechanics provides engineers with a broad portfolio of technically leading technologies for the entire application spectrum of fluid simulation, with which they can reliably determine the influence of fluid flows, even with complex interactions between different physical influencing factors and moving geometries.</t>
   </si>
   <si>
-    <t xml:space="preserve">KNIME, the "Konstanz Information Miner", is free software for interactive data analysis. Thanks to its modular pipelining concept, KNIME enables the integration of numerous machine learning and data mining methods.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">free version available, paid versions for professional applications. For the open source part: Each module is published under its own license.</t>
+    <t xml:space="preserve">KNIME, the “Konstanz Information Miner”, is free software for interactive data analysis. Thanks to its modular pipelining concept, KNIME enables the integration of numerous machine learning and data mining methods.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">free version available, paid versions for professional applications. For the open-source part: Each module is published under its own license.</t>
   </si>
   <si>
     <t xml:space="preserve">E2M2 (European Electricity Market Model) is a basic electricity market model developed with the aim of minimizing system costs in the European electricity market.</t>
@@ -4095,6 +4110,9 @@
   </si>
   <si>
     <t xml:space="preserve">RFEM is a 3D FEM software for the structural analysis and design of steel, reinforced concrete, timber, glass and membrane structures, for plant and mechanical engineering as well as for dynamic analyses.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">THERAKLES</t>
   </si>
   <si>
     <t xml:space="preserve">The THERAKLES simulation program calculates the dynamic thermal or hygrothermal behavior of rooms and buildings. It is a calculation tool for planning engineers and architects in the field of building physics, building climate and technical building equipment.</t>
@@ -4139,10 +4157,10 @@
     <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
     <numFmt numFmtId="166" formatCode="dd/mm/yy"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -4165,7 +4183,7 @@
     <font>
       <b val="true"/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -4173,16 +4191,10 @@
     <font>
       <u val="single"/>
       <sz val="11"/>
-      <color theme="10"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -4237,7 +4249,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -4262,10 +4274,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4279,183 +4287,8 @@
 </styleSheet>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
-  <a:themeElements>
-    <a:clrScheme name="Office">
-      <a:dk1>
-        <a:srgbClr val="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:srgbClr val="ffffff"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="1f497d"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="eeece1"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="4f81bd"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="c0504d"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="9bbb59"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="8064a2"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="4bacc6"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="f79646"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0000ff"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="800080"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Cambria" pitchFamily="0" charset="1"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Calibri" pitchFamily="0" charset="1"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme>
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill>
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="35000">
-              <a:schemeClr val="phClr">
-                <a:tint val="37000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
-        </a:gradFill>
-        <a:gradFill>
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:shade val="51000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="80000">
-              <a:schemeClr val="phClr">
-                <a:shade val="93000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="16200000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
-        </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill>
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="40000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="40000">
-              <a:schemeClr val="phClr">
-                <a:tint val="45000"/>
-                <a:shade val="99000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="20000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
-          </a:path>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
-        </a:gradFill>
-        <a:gradFill>
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="80000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="30000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-          </a:path>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
-        </a:gradFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-</a:theme>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -4465,7 +4298,7 @@
       <selection pane="topLeft" activeCell="W5" activeCellId="0" sqref="W5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -12745,17 +12578,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:AD1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="W5" activeCellId="0" sqref="W5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A110" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L138" activeCellId="0" sqref="L138"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -13087,7 +12920,7 @@
       <c r="R5" s="2" t="s">
         <v>1101</v>
       </c>
-      <c r="W5" s="6" t="s">
+      <c r="W5" s="2" t="s">
         <v>90</v>
       </c>
       <c r="X5" s="2" t="n">
@@ -13462,6 +13295,9 @@
       <c r="I11" s="2" t="s">
         <v>1072</v>
       </c>
+      <c r="J11" s="0" t="s">
+        <v>1132</v>
+      </c>
       <c r="K11" s="2" t="s">
         <v>59</v>
       </c>
@@ -13507,7 +13343,7 @@
         <v>162</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>1096</v>
@@ -13572,10 +13408,10 @@
         <v>170</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>1133</v>
+        <v>1134</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>1134</v>
+        <v>1135</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>173</v>
@@ -13602,7 +13438,7 @@
         <v>1074</v>
       </c>
       <c r="P13" s="2" t="s">
-        <v>1135</v>
+        <v>1136</v>
       </c>
       <c r="Q13" s="2" t="s">
         <v>175</v>
@@ -13640,7 +13476,7 @@
         <v>181</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>1136</v>
+        <v>1137</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>1080</v>
@@ -13649,16 +13485,16 @@
         <v>183</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>1137</v>
+        <v>1138</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>1138</v>
+        <v>1139</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>1139</v>
+        <v>1140</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>1140</v>
+        <v>1141</v>
       </c>
       <c r="K14" s="2" t="s">
         <v>188</v>
@@ -13670,10 +13506,10 @@
         <v>190</v>
       </c>
       <c r="N14" s="2" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="O14" s="2" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="Q14" s="2" t="s">
         <v>1076</v>
@@ -13685,7 +13521,7 @@
         <v>193</v>
       </c>
       <c r="T14" s="2" t="s">
-        <v>1143</v>
+        <v>1144</v>
       </c>
       <c r="X14" s="2" t="n">
         <v>1</v>
@@ -13708,7 +13544,7 @@
         <v>198</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>1144</v>
+        <v>1145</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>1080</v>
@@ -13720,7 +13556,7 @@
         <v>1092</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>1145</v>
+        <v>1146</v>
       </c>
       <c r="H15" s="2" t="s">
         <v>1083</v>
@@ -13735,7 +13571,7 @@
         <v>1094</v>
       </c>
       <c r="O15" s="2" t="s">
-        <v>1146</v>
+        <v>1147</v>
       </c>
       <c r="P15" s="2" t="s">
         <v>1087</v>
@@ -13770,7 +13606,7 @@
         <v>206</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>1147</v>
+        <v>1148</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>1080</v>
@@ -13779,7 +13615,7 @@
         <v>208</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>1148</v>
+        <v>1149</v>
       </c>
       <c r="G16" s="2" t="s">
         <v>1070</v>
@@ -13826,7 +13662,7 @@
         <v>213</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>1149</v>
+        <v>1150</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>1068</v>
@@ -13838,7 +13674,7 @@
         <v>1103</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>1138</v>
+        <v>1139</v>
       </c>
       <c r="H17" s="2" t="s">
         <v>1083</v>
@@ -13853,10 +13689,10 @@
         <v>1073</v>
       </c>
       <c r="O17" s="2" t="s">
-        <v>1146</v>
+        <v>1147</v>
       </c>
       <c r="P17" s="2" t="s">
-        <v>1150</v>
+        <v>1151</v>
       </c>
       <c r="Q17" s="2" t="s">
         <v>1076</v>
@@ -13888,7 +13724,7 @@
         <v>220</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>1151</v>
+        <v>1152</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>1096</v>
@@ -13956,10 +13792,10 @@
         <v>230</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>1152</v>
+        <v>1153</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>1153</v>
+        <v>1154</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>71</v>
@@ -14018,7 +13854,7 @@
         <v>238</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>1154</v>
+        <v>1155</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>1096</v>
@@ -14089,7 +13925,7 @@
         <v>246</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>1155</v>
+        <v>1156</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>1096</v>
@@ -14104,7 +13940,7 @@
         <v>1070</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>1156</v>
+        <v>1157</v>
       </c>
       <c r="I21" s="2" t="s">
         <v>1084</v>
@@ -14137,7 +13973,7 @@
         <v>251</v>
       </c>
       <c r="T21" s="2" t="s">
-        <v>1157</v>
+        <v>1158</v>
       </c>
       <c r="W21" s="2" t="s">
         <v>253</v>
@@ -14163,7 +13999,7 @@
         <v>257</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>1158</v>
+        <v>1159</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>1096</v>
@@ -14234,10 +14070,10 @@
         <v>268</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>1159</v>
+        <v>1160</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>1160</v>
+        <v>1161</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>271</v>
@@ -14249,16 +14085,16 @@
         <v>1070</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>1161</v>
+        <v>1162</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>1140</v>
+        <v>1141</v>
       </c>
       <c r="N23" s="2" t="s">
         <v>273</v>
       </c>
       <c r="O23" s="2" t="s">
-        <v>1162</v>
+        <v>1163</v>
       </c>
       <c r="Q23" s="2" t="s">
         <v>1113</v>
@@ -14287,7 +14123,7 @@
         <v>278</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>1163</v>
+        <v>1164</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>1068</v>
@@ -14296,7 +14132,7 @@
         <v>280</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>1164</v>
+        <v>1165</v>
       </c>
       <c r="G24" s="2" t="s">
         <v>1082</v>
@@ -14352,7 +14188,7 @@
         <v>288</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>1165</v>
+        <v>1166</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>1096</v>
@@ -14370,7 +14206,7 @@
         <v>1083</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>1166</v>
+        <v>1167</v>
       </c>
       <c r="K25" s="2" t="s">
         <v>292</v>
@@ -14400,7 +14236,7 @@
         <v>165</v>
       </c>
       <c r="T25" s="2" t="s">
-        <v>1167</v>
+        <v>1168</v>
       </c>
       <c r="V25" s="2" t="s">
         <v>295</v>
@@ -14426,7 +14262,7 @@
         <v>298</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>1168</v>
+        <v>1169</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>1096</v>
@@ -14435,7 +14271,7 @@
         <v>300</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>1164</v>
+        <v>1165</v>
       </c>
       <c r="G26" s="2" t="s">
         <v>1070</v>
@@ -14462,7 +14298,7 @@
         <v>1077</v>
       </c>
       <c r="T26" s="2" t="s">
-        <v>1169</v>
+        <v>1170</v>
       </c>
       <c r="X26" s="2" t="n">
         <v>1</v>
@@ -14485,7 +14321,7 @@
         <v>304</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>1170</v>
+        <v>1171</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>1080</v>
@@ -14524,7 +14360,7 @@
         <v>76</v>
       </c>
       <c r="T27" s="2" t="s">
-        <v>1171</v>
+        <v>1172</v>
       </c>
       <c r="W27" s="2" t="s">
         <v>308</v>
@@ -14544,13 +14380,13 @@
     </row>
     <row r="28" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="s">
-        <v>310</v>
+        <v>1173</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>311</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>1172</v>
+        <v>1174</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>1068</v>
@@ -14559,10 +14395,10 @@
         <v>313</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>1173</v>
+        <v>1175</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>1145</v>
+        <v>1146</v>
       </c>
       <c r="H28" s="2" t="s">
         <v>1099</v>
@@ -14618,7 +14454,7 @@
         <v>321</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>1174</v>
+        <v>1176</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>1096</v>
@@ -14686,7 +14522,7 @@
         <v>330</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>1175</v>
+        <v>1177</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>1091</v>
@@ -14751,7 +14587,7 @@
         <v>338</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>1176</v>
+        <v>1178</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>1096</v>
@@ -14816,7 +14652,7 @@
         <v>347</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>1177</v>
+        <v>1179</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>1096</v>
@@ -14828,7 +14664,7 @@
         <v>1125</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>1138</v>
+        <v>1139</v>
       </c>
       <c r="H32" s="2" t="s">
         <v>1083</v>
@@ -14837,7 +14673,7 @@
         <v>1126</v>
       </c>
       <c r="J32" s="2" t="s">
-        <v>1178</v>
+        <v>1180</v>
       </c>
       <c r="K32" s="2" t="s">
         <v>59</v>
@@ -14849,7 +14685,7 @@
         <v>1074</v>
       </c>
       <c r="P32" s="2" t="s">
-        <v>1179</v>
+        <v>1181</v>
       </c>
       <c r="Q32" s="2" t="s">
         <v>1076</v>
@@ -14887,7 +14723,7 @@
         <v>358</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>1180</v>
+        <v>1182</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>1068</v>
@@ -14908,7 +14744,7 @@
         <v>1126</v>
       </c>
       <c r="J33" s="2" t="s">
-        <v>1181</v>
+        <v>1183</v>
       </c>
       <c r="K33" s="2" t="s">
         <v>116</v>
@@ -14920,7 +14756,7 @@
         <v>1100</v>
       </c>
       <c r="O33" s="2" t="s">
-        <v>1146</v>
+        <v>1147</v>
       </c>
       <c r="P33" s="2" t="s">
         <v>1116</v>
@@ -14958,10 +14794,10 @@
         <v>367</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>1182</v>
+        <v>1184</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>1160</v>
+        <v>1161</v>
       </c>
       <c r="E34" s="2" t="s">
         <v>271</v>
@@ -14973,16 +14809,16 @@
         <v>1104</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>1161</v>
+        <v>1162</v>
       </c>
       <c r="I34" s="2" t="s">
-        <v>1140</v>
+        <v>1141</v>
       </c>
       <c r="N34" s="2" t="s">
         <v>1108</v>
       </c>
       <c r="O34" s="2" t="s">
-        <v>1162</v>
+        <v>1163</v>
       </c>
       <c r="Q34" s="2" t="s">
         <v>1113</v>
@@ -14993,9 +14829,7 @@
       <c r="X34" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="Z34" s="2" t="s">
-        <v>1113</v>
-      </c>
+      <c r="Z34" s="2"/>
       <c r="AA34" s="2" t="n">
         <v>5</v>
       </c>
@@ -15011,7 +14845,7 @@
         <v>371</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>1183</v>
+        <v>1185</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>1096</v>
@@ -15020,7 +14854,7 @@
         <v>373</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>1137</v>
+        <v>1138</v>
       </c>
       <c r="G35" s="2" t="s">
         <v>1070</v>
@@ -15038,7 +14872,7 @@
         <v>1074</v>
       </c>
       <c r="P35" s="2" t="s">
-        <v>1184</v>
+        <v>1186</v>
       </c>
       <c r="Q35" s="2" t="s">
         <v>1113</v>
@@ -15067,7 +14901,7 @@
         <v>378</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>1185</v>
+        <v>1187</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>1068</v>
@@ -15091,16 +14925,16 @@
         <v>1108</v>
       </c>
       <c r="O36" s="2" t="s">
-        <v>1146</v>
+        <v>1147</v>
       </c>
       <c r="P36" s="2" t="s">
-        <v>1186</v>
+        <v>1188</v>
       </c>
       <c r="Q36" s="2" t="s">
         <v>1113</v>
       </c>
       <c r="R36" s="2" t="s">
-        <v>1187</v>
+        <v>1189</v>
       </c>
       <c r="W36" s="2" t="s">
         <v>384</v>
@@ -15120,7 +14954,7 @@
         <v>387</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>1188</v>
+        <v>1190</v>
       </c>
       <c r="D37" s="2" t="s">
         <v>1096</v>
@@ -15129,7 +14963,7 @@
         <v>389</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>1189</v>
+        <v>1191</v>
       </c>
       <c r="G37" s="2" t="s">
         <v>1120</v>
@@ -15185,7 +15019,7 @@
         <v>395</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>1190</v>
+        <v>1192</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>1096</v>
@@ -15194,7 +15028,7 @@
         <v>397</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>1148</v>
+        <v>1149</v>
       </c>
       <c r="G38" s="2" t="s">
         <v>1070</v>
@@ -15215,7 +15049,7 @@
         <v>1074</v>
       </c>
       <c r="P38" s="2" t="s">
-        <v>1191</v>
+        <v>1193</v>
       </c>
       <c r="Q38" s="2" t="s">
         <v>399</v>
@@ -15227,7 +15061,7 @@
         <v>400</v>
       </c>
       <c r="U38" s="2" t="s">
-        <v>1192</v>
+        <v>1194</v>
       </c>
       <c r="V38" s="2" t="s">
         <v>402</v>
@@ -15256,7 +15090,7 @@
         <v>407</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>1193</v>
+        <v>1195</v>
       </c>
       <c r="D39" s="2" t="s">
         <v>1096</v>
@@ -15292,7 +15126,7 @@
         <v>1077</v>
       </c>
       <c r="U39" s="2" t="s">
-        <v>1194</v>
+        <v>1196</v>
       </c>
       <c r="W39" s="2" t="s">
         <v>411</v>
@@ -15318,7 +15152,7 @@
         <v>415</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>1195</v>
+        <v>1197</v>
       </c>
       <c r="D40" s="2" t="s">
         <v>1068</v>
@@ -15339,7 +15173,7 @@
         <v>1126</v>
       </c>
       <c r="J40" s="2" t="s">
-        <v>1181</v>
+        <v>1183</v>
       </c>
       <c r="K40" s="2" t="s">
         <v>116</v>
@@ -15351,10 +15185,10 @@
         <v>1100</v>
       </c>
       <c r="O40" s="2" t="s">
-        <v>1146</v>
+        <v>1147</v>
       </c>
       <c r="P40" s="2" t="s">
-        <v>1179</v>
+        <v>1181</v>
       </c>
       <c r="Q40" s="2" t="s">
         <v>1076</v>
@@ -15366,7 +15200,7 @@
         <v>165</v>
       </c>
       <c r="U40" s="2" t="s">
-        <v>1196</v>
+        <v>1198</v>
       </c>
       <c r="V40" s="2" t="s">
         <v>420</v>
@@ -15392,10 +15226,10 @@
         <v>423</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>1197</v>
+        <v>1199</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>1160</v>
+        <v>1161</v>
       </c>
       <c r="E41" s="2" t="s">
         <v>425</v>
@@ -15407,19 +15241,19 @@
         <v>1070</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>1161</v>
+        <v>1162</v>
       </c>
       <c r="I41" s="2" t="s">
-        <v>1140</v>
+        <v>1141</v>
       </c>
       <c r="J41" s="2" t="s">
-        <v>1198</v>
+        <v>1200</v>
       </c>
       <c r="N41" s="2" t="s">
         <v>1108</v>
       </c>
       <c r="O41" s="2" t="s">
-        <v>1162</v>
+        <v>1163</v>
       </c>
       <c r="P41" s="2" t="s">
         <v>1105</v>
@@ -15451,7 +15285,7 @@
         <v>429</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>1199</v>
+        <v>1201</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>1068</v>
@@ -15463,7 +15297,7 @@
         <v>1125</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>1138</v>
+        <v>1139</v>
       </c>
       <c r="H42" s="2" t="s">
         <v>1083</v>
@@ -15472,7 +15306,7 @@
         <v>1126</v>
       </c>
       <c r="J42" s="2" t="s">
-        <v>1181</v>
+        <v>1183</v>
       </c>
       <c r="K42" s="2" t="s">
         <v>116</v>
@@ -15516,7 +15350,7 @@
         <v>434</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>1200</v>
+        <v>1202</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>1068</v>
@@ -15581,10 +15415,10 @@
         <v>442</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>1201</v>
+        <v>1203</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>1202</v>
+        <v>1204</v>
       </c>
       <c r="E44" s="2" t="s">
         <v>445</v>
@@ -15593,7 +15427,7 @@
         <v>1103</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>1203</v>
+        <v>1205</v>
       </c>
       <c r="H44" s="2" t="s">
         <v>1071</v>
@@ -15614,13 +15448,13 @@
         <v>1074</v>
       </c>
       <c r="P44" s="2" t="s">
-        <v>1150</v>
+        <v>1151</v>
       </c>
       <c r="Q44" s="2" t="s">
         <v>448</v>
       </c>
       <c r="R44" s="2" t="s">
-        <v>1187</v>
+        <v>1189</v>
       </c>
       <c r="V44" s="2" t="s">
         <v>449</v>
@@ -15646,7 +15480,7 @@
         <v>452</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>1204</v>
+        <v>1206</v>
       </c>
       <c r="D45" s="2" t="s">
         <v>1068</v>
@@ -15655,7 +15489,7 @@
         <v>454</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>1173</v>
+        <v>1175</v>
       </c>
       <c r="G45" s="2" t="s">
         <v>1120</v>
@@ -15664,7 +15498,7 @@
         <v>1071</v>
       </c>
       <c r="I45" s="2" t="s">
-        <v>1140</v>
+        <v>1141</v>
       </c>
       <c r="N45" s="2" t="s">
         <v>1108</v>
@@ -15679,7 +15513,7 @@
         <v>1113</v>
       </c>
       <c r="R45" s="2" t="s">
-        <v>1187</v>
+        <v>1189</v>
       </c>
       <c r="AD45" s="2" t="s">
         <v>455</v>
@@ -15693,7 +15527,7 @@
         <v>457</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>1205</v>
+        <v>1207</v>
       </c>
       <c r="D46" s="2" t="s">
         <v>1096</v>
@@ -15702,7 +15536,7 @@
         <v>459</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>1206</v>
+        <v>1208</v>
       </c>
       <c r="G46" s="2" t="s">
         <v>1115</v>
@@ -15711,7 +15545,7 @@
         <v>1093</v>
       </c>
       <c r="I46" s="2" t="s">
-        <v>1207</v>
+        <v>1209</v>
       </c>
       <c r="J46" s="2" t="s">
         <v>462</v>
@@ -15738,7 +15572,7 @@
         <v>464</v>
       </c>
       <c r="T46" s="2" t="s">
-        <v>1208</v>
+        <v>1210</v>
       </c>
       <c r="X46" s="2" t="n">
         <v>1</v>
@@ -15761,7 +15595,7 @@
         <v>468</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>1209</v>
+        <v>1211</v>
       </c>
       <c r="D47" s="2" t="s">
         <v>1068</v>
@@ -15779,10 +15613,10 @@
         <v>1099</v>
       </c>
       <c r="I47" s="2" t="s">
-        <v>1210</v>
+        <v>1212</v>
       </c>
       <c r="J47" s="2" t="s">
-        <v>1211</v>
+        <v>1213</v>
       </c>
       <c r="K47" s="2" t="s">
         <v>59</v>
@@ -15803,7 +15637,7 @@
         <v>76</v>
       </c>
       <c r="T47" s="2" t="s">
-        <v>1212</v>
+        <v>1214</v>
       </c>
       <c r="W47" s="2" t="s">
         <v>334</v>
@@ -15812,7 +15646,7 @@
         <v>1</v>
       </c>
       <c r="Z47" s="2" t="s">
-        <v>1213</v>
+        <v>1215</v>
       </c>
       <c r="AA47" s="2" t="n">
         <v>5</v>
@@ -15829,7 +15663,7 @@
         <v>477</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>1214</v>
+        <v>1216</v>
       </c>
       <c r="D48" s="2" t="s">
         <v>1068</v>
@@ -15841,7 +15675,7 @@
         <v>1103</v>
       </c>
       <c r="G48" s="2" t="s">
-        <v>1138</v>
+        <v>1139</v>
       </c>
       <c r="H48" s="2" t="s">
         <v>1099</v>
@@ -15850,7 +15684,7 @@
         <v>1126</v>
       </c>
       <c r="J48" s="2" t="s">
-        <v>1215</v>
+        <v>1183</v>
       </c>
       <c r="K48" s="2" t="s">
         <v>116</v>
@@ -15862,10 +15696,10 @@
         <v>1100</v>
       </c>
       <c r="O48" s="2" t="s">
-        <v>1146</v>
+        <v>1147</v>
       </c>
       <c r="P48" s="2" t="s">
-        <v>1150</v>
+        <v>1151</v>
       </c>
       <c r="Q48" s="2" t="s">
         <v>480</v>
@@ -15900,10 +15734,10 @@
         <v>484</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>1216</v>
+        <v>1217</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>1217</v>
+        <v>1218</v>
       </c>
       <c r="E49" s="2" t="s">
         <v>271</v>
@@ -15912,19 +15746,19 @@
         <v>1104</v>
       </c>
       <c r="G49" s="2" t="s">
-        <v>1218</v>
+        <v>1219</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>1161</v>
+        <v>1162</v>
       </c>
       <c r="I49" s="2" t="s">
-        <v>1140</v>
+        <v>1141</v>
       </c>
       <c r="N49" s="2" t="s">
         <v>1108</v>
       </c>
       <c r="O49" s="2" t="s">
-        <v>1162</v>
+        <v>1163</v>
       </c>
       <c r="Q49" s="2" t="s">
         <v>1113</v>
@@ -15950,7 +15784,7 @@
         <v>490</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>1219</v>
+        <v>1220</v>
       </c>
       <c r="D50" s="2" t="s">
         <v>1096</v>
@@ -15959,10 +15793,10 @@
         <v>492</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>1220</v>
+        <v>1221</v>
       </c>
       <c r="G50" s="2" t="s">
-        <v>1138</v>
+        <v>1139</v>
       </c>
       <c r="H50" s="2" t="s">
         <v>1083</v>
@@ -15983,7 +15817,7 @@
         <v>1074</v>
       </c>
       <c r="P50" s="2" t="s">
-        <v>1221</v>
+        <v>1222</v>
       </c>
       <c r="Q50" s="2" t="s">
         <v>1076</v>
@@ -16010,15 +15844,15 @@
         <v>498</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="2" t="s">
-        <v>499</v>
+        <v>1223</v>
       </c>
       <c r="B51" s="3" t="s">
         <v>500</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>1222</v>
+        <v>1224</v>
       </c>
       <c r="D51" s="2" t="s">
         <v>1096</v>
@@ -16074,7 +15908,7 @@
         <v>507</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>1223</v>
+        <v>1225</v>
       </c>
       <c r="D52" s="2" t="s">
         <v>1068</v>
@@ -16083,19 +15917,19 @@
         <v>140</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>1206</v>
+        <v>1208</v>
       </c>
       <c r="G52" s="2" t="s">
-        <v>1138</v>
+        <v>1139</v>
       </c>
       <c r="H52" s="2" t="s">
         <v>1099</v>
       </c>
       <c r="I52" s="2" t="s">
-        <v>1140</v>
+        <v>1141</v>
       </c>
       <c r="J52" s="2" t="s">
-        <v>1224</v>
+        <v>1226</v>
       </c>
       <c r="K52" s="2" t="s">
         <v>116</v>
@@ -16107,7 +15941,7 @@
         <v>1074</v>
       </c>
       <c r="P52" s="2" t="s">
-        <v>1150</v>
+        <v>1151</v>
       </c>
       <c r="Q52" s="2" t="s">
         <v>1076</v>
@@ -16119,7 +15953,7 @@
         <v>118</v>
       </c>
       <c r="T52" s="2" t="s">
-        <v>1225</v>
+        <v>1227</v>
       </c>
       <c r="W52" s="2" t="s">
         <v>363</v>
@@ -16145,7 +15979,7 @@
         <v>513</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>1226</v>
+        <v>1228</v>
       </c>
       <c r="D53" s="2" t="s">
         <v>1096</v>
@@ -16166,7 +16000,7 @@
         <v>1081</v>
       </c>
       <c r="J53" s="2" t="s">
-        <v>1227</v>
+        <v>1229</v>
       </c>
       <c r="N53" s="2" t="s">
         <v>1086</v>
@@ -16184,7 +16018,7 @@
         <v>1077</v>
       </c>
       <c r="T53" s="2" t="s">
-        <v>1228</v>
+        <v>1230</v>
       </c>
       <c r="W53" s="2" t="s">
         <v>519</v>
@@ -16210,10 +16044,10 @@
         <v>523</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>1229</v>
+        <v>1231</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>1230</v>
+        <v>1232</v>
       </c>
       <c r="E54" s="2" t="s">
         <v>526</v>
@@ -16228,7 +16062,7 @@
         <v>1121</v>
       </c>
       <c r="I54" s="2" t="s">
-        <v>1140</v>
+        <v>1141</v>
       </c>
       <c r="N54" s="2" t="s">
         <v>1108</v>
@@ -16237,7 +16071,7 @@
         <v>1074</v>
       </c>
       <c r="P54" s="2" t="s">
-        <v>1231</v>
+        <v>1233</v>
       </c>
       <c r="Q54" s="2" t="s">
         <v>1076</v>
@@ -16269,7 +16103,7 @@
         <v>531</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>1232</v>
+        <v>1234</v>
       </c>
       <c r="D55" s="2" t="s">
         <v>1096</v>
@@ -16281,7 +16115,7 @@
         <v>1069</v>
       </c>
       <c r="G55" s="2" t="s">
-        <v>1145</v>
+        <v>1146</v>
       </c>
       <c r="H55" s="2" t="s">
         <v>1093</v>
@@ -16299,7 +16133,7 @@
         <v>1074</v>
       </c>
       <c r="P55" s="2" t="s">
-        <v>1179</v>
+        <v>1181</v>
       </c>
       <c r="Q55" s="2" t="s">
         <v>1076</v>
@@ -16308,7 +16142,7 @@
         <v>1077</v>
       </c>
       <c r="U55" s="2" t="s">
-        <v>1233</v>
+        <v>1235</v>
       </c>
       <c r="V55" s="2" t="s">
         <v>534</v>
@@ -16337,19 +16171,19 @@
         <v>538</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>1234</v>
+        <v>1236</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>1217</v>
+        <v>1218</v>
       </c>
       <c r="E56" s="2" t="s">
         <v>540</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>1235</v>
+        <v>1237</v>
       </c>
       <c r="G56" s="2" t="s">
-        <v>1145</v>
+        <v>1146</v>
       </c>
       <c r="H56" s="2" t="s">
         <v>1121</v>
@@ -16361,7 +16195,7 @@
         <v>1108</v>
       </c>
       <c r="O56" s="2" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="P56" s="2" t="s">
         <v>1105</v>
@@ -16396,7 +16230,7 @@
         <v>545</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>1236</v>
+        <v>1238</v>
       </c>
       <c r="D57" s="2" t="s">
         <v>1096</v>
@@ -16423,7 +16257,7 @@
         <v>1074</v>
       </c>
       <c r="P57" s="2" t="s">
-        <v>1237</v>
+        <v>1239</v>
       </c>
       <c r="Q57" s="2" t="s">
         <v>1113</v>
@@ -16432,7 +16266,7 @@
         <v>1077</v>
       </c>
       <c r="T57" s="2" t="s">
-        <v>1238</v>
+        <v>1240</v>
       </c>
       <c r="W57" s="2" t="s">
         <v>550</v>
@@ -16458,7 +16292,7 @@
         <v>553</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>1239</v>
+        <v>1241</v>
       </c>
       <c r="D58" s="2" t="s">
         <v>1068</v>
@@ -16467,7 +16301,7 @@
         <v>555</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>1240</v>
+        <v>1242</v>
       </c>
       <c r="G58" s="2" t="s">
         <v>1120</v>
@@ -16488,7 +16322,7 @@
         <v>1074</v>
       </c>
       <c r="P58" s="2" t="s">
-        <v>1221</v>
+        <v>1222</v>
       </c>
       <c r="Q58" s="2" t="s">
         <v>558</v>
@@ -16506,7 +16340,7 @@
         <v>1</v>
       </c>
       <c r="Z58" s="2" t="s">
-        <v>1241</v>
+        <v>1243</v>
       </c>
       <c r="AA58" s="2" t="n">
         <v>5</v>
@@ -16523,7 +16357,7 @@
         <v>564</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>1242</v>
+        <v>1244</v>
       </c>
       <c r="D59" s="2" t="s">
         <v>1096</v>
@@ -16550,7 +16384,7 @@
         <v>1074</v>
       </c>
       <c r="P59" s="2" t="s">
-        <v>1179</v>
+        <v>1181</v>
       </c>
       <c r="Q59" s="2" t="s">
         <v>567</v>
@@ -16559,7 +16393,7 @@
         <v>1077</v>
       </c>
       <c r="T59" s="2" t="s">
-        <v>1243</v>
+        <v>1245</v>
       </c>
       <c r="V59" s="2" t="s">
         <v>569</v>
@@ -16579,7 +16413,7 @@
         <v>573</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>1244</v>
+        <v>1246</v>
       </c>
       <c r="D60" s="2" t="s">
         <v>1080</v>
@@ -16594,7 +16428,7 @@
         <v>1120</v>
       </c>
       <c r="H60" s="2" t="s">
-        <v>1245</v>
+        <v>1247</v>
       </c>
       <c r="I60" s="2" t="s">
         <v>1126</v>
@@ -16621,7 +16455,7 @@
         <v>579</v>
       </c>
       <c r="T60" s="2" t="s">
-        <v>1246</v>
+        <v>1248</v>
       </c>
       <c r="V60" s="2" t="s">
         <v>581</v>
@@ -16650,7 +16484,7 @@
         <v>585</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>1247</v>
+        <v>1249</v>
       </c>
       <c r="D61" s="2" t="s">
         <v>1068</v>
@@ -16715,10 +16549,10 @@
         <v>590</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>1248</v>
+        <v>1250</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>1202</v>
+        <v>1204</v>
       </c>
       <c r="E62" s="2" t="s">
         <v>592</v>
@@ -16742,7 +16576,7 @@
         <v>1074</v>
       </c>
       <c r="P62" s="2" t="s">
-        <v>1221</v>
+        <v>1222</v>
       </c>
       <c r="Q62" s="2" t="s">
         <v>1113</v>
@@ -16771,7 +16605,7 @@
         <v>596</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>1249</v>
+        <v>1251</v>
       </c>
       <c r="D63" s="2" t="s">
         <v>1068</v>
@@ -16839,7 +16673,7 @@
         <v>604</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>1250</v>
+        <v>1252</v>
       </c>
       <c r="D64" s="2" t="s">
         <v>1080</v>
@@ -16848,10 +16682,10 @@
         <v>606</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>1235</v>
+        <v>1237</v>
       </c>
       <c r="G64" s="2" t="s">
-        <v>1145</v>
+        <v>1146</v>
       </c>
       <c r="H64" s="2" t="s">
         <v>1083</v>
@@ -16866,7 +16700,7 @@
         <v>1094</v>
       </c>
       <c r="O64" s="2" t="s">
-        <v>1146</v>
+        <v>1147</v>
       </c>
       <c r="P64" s="2" t="s">
         <v>1075</v>
@@ -16901,31 +16735,31 @@
         <v>610</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>1251</v>
+        <v>1253</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>1153</v>
+        <v>1154</v>
       </c>
       <c r="E65" s="2" t="s">
         <v>612</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>1252</v>
+        <v>1254</v>
       </c>
       <c r="G65" s="2" t="s">
         <v>1120</v>
       </c>
       <c r="H65" s="2" t="s">
-        <v>1253</v>
+        <v>1255</v>
       </c>
       <c r="I65" s="2" t="s">
-        <v>1140</v>
+        <v>1141</v>
       </c>
       <c r="N65" s="2" t="s">
         <v>1108</v>
       </c>
       <c r="O65" s="2" t="s">
-        <v>1146</v>
+        <v>1147</v>
       </c>
       <c r="P65" s="2" t="s">
         <v>1116</v>
@@ -16934,7 +16768,7 @@
         <v>1113</v>
       </c>
       <c r="R65" s="2" t="s">
-        <v>1187</v>
+        <v>1189</v>
       </c>
       <c r="W65" s="2" t="s">
         <v>615</v>
@@ -16951,7 +16785,7 @@
         <v>618</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>1254</v>
+        <v>1256</v>
       </c>
       <c r="D66" s="2" t="s">
         <v>1068</v>
@@ -16960,7 +16794,7 @@
         <v>620</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>1255</v>
+        <v>1257</v>
       </c>
       <c r="G66" s="2" t="s">
         <v>1070</v>
@@ -16969,16 +16803,16 @@
         <v>1121</v>
       </c>
       <c r="I66" s="2" t="s">
-        <v>1140</v>
+        <v>1141</v>
       </c>
       <c r="N66" s="2" t="s">
         <v>1108</v>
       </c>
       <c r="O66" s="2" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="P66" s="2" t="s">
-        <v>1150</v>
+        <v>1151</v>
       </c>
       <c r="Q66" s="2" t="s">
         <v>1113</v>
@@ -17004,7 +16838,7 @@
         <v>624</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>1256</v>
+        <v>1258</v>
       </c>
       <c r="D67" s="2" t="s">
         <v>1091</v>
@@ -17013,7 +16847,7 @@
         <v>626</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>1206</v>
+        <v>1208</v>
       </c>
       <c r="G67" s="2" t="s">
         <v>1104</v>
@@ -17031,7 +16865,7 @@
         <v>1074</v>
       </c>
       <c r="P67" s="2" t="s">
-        <v>1191</v>
+        <v>1193</v>
       </c>
       <c r="Q67" s="2" t="s">
         <v>627</v>
@@ -17040,7 +16874,7 @@
         <v>1077</v>
       </c>
       <c r="U67" s="2" t="s">
-        <v>1257</v>
+        <v>1259</v>
       </c>
       <c r="W67" s="2" t="s">
         <v>570</v>
@@ -17066,7 +16900,7 @@
         <v>632</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>1258</v>
+        <v>1260</v>
       </c>
       <c r="D68" s="2" t="s">
         <v>1068</v>
@@ -17075,10 +16909,10 @@
         <v>634</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>1148</v>
+        <v>1149</v>
       </c>
       <c r="G68" s="2" t="s">
-        <v>1203</v>
+        <v>1205</v>
       </c>
       <c r="H68" s="2" t="s">
         <v>1099</v>
@@ -17093,7 +16927,7 @@
         <v>1074</v>
       </c>
       <c r="P68" s="2" t="s">
-        <v>1150</v>
+        <v>1151</v>
       </c>
       <c r="Q68" s="2" t="s">
         <v>636</v>
@@ -17102,7 +16936,7 @@
         <v>275</v>
       </c>
       <c r="T68" s="2" t="s">
-        <v>1259</v>
+        <v>1261</v>
       </c>
       <c r="W68" s="2" t="s">
         <v>550</v>
@@ -17125,16 +16959,16 @@
         <v>640</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>1260</v>
+        <v>1262</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>1153</v>
+        <v>1154</v>
       </c>
       <c r="E69" s="2" t="s">
         <v>642</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>1148</v>
+        <v>1149</v>
       </c>
       <c r="G69" s="2" t="s">
         <v>1070</v>
@@ -17181,7 +17015,7 @@
         <v>645</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>1261</v>
+        <v>1263</v>
       </c>
       <c r="D70" s="2" t="s">
         <v>1091</v>
@@ -17190,13 +17024,13 @@
         <v>647</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>1262</v>
+        <v>1264</v>
       </c>
       <c r="G70" s="2" t="s">
-        <v>1263</v>
+        <v>1265</v>
       </c>
       <c r="H70" s="2" t="s">
-        <v>1161</v>
+        <v>1162</v>
       </c>
       <c r="I70" s="2" t="s">
         <v>1072</v>
@@ -17205,7 +17039,7 @@
         <v>1108</v>
       </c>
       <c r="O70" s="2" t="s">
-        <v>1162</v>
+        <v>1163</v>
       </c>
       <c r="Q70" s="2" t="s">
         <v>1076</v>
@@ -17234,7 +17068,7 @@
         <v>652</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>1264</v>
+        <v>1266</v>
       </c>
       <c r="D71" s="2" t="s">
         <v>1080</v>
@@ -17249,10 +17083,10 @@
         <v>1070</v>
       </c>
       <c r="H71" s="2" t="s">
-        <v>1253</v>
+        <v>1255</v>
       </c>
       <c r="I71" s="2" t="s">
-        <v>1140</v>
+        <v>1141</v>
       </c>
       <c r="N71" s="2" t="s">
         <v>1073</v>
@@ -17267,10 +17101,10 @@
         <v>1113</v>
       </c>
       <c r="R71" s="2" t="s">
-        <v>1187</v>
+        <v>1189</v>
       </c>
       <c r="U71" s="2" t="s">
-        <v>1265</v>
+        <v>1267</v>
       </c>
       <c r="W71" s="2" t="s">
         <v>656</v>
@@ -17290,7 +17124,7 @@
         <v>659</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>1266</v>
+        <v>1268</v>
       </c>
       <c r="D72" s="2" t="s">
         <v>1080</v>
@@ -17299,13 +17133,13 @@
         <v>661</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>1267</v>
+        <v>1269</v>
       </c>
       <c r="G72" s="2" t="s">
         <v>1082</v>
       </c>
       <c r="H72" s="2" t="s">
-        <v>1139</v>
+        <v>1140</v>
       </c>
       <c r="I72" s="2" t="s">
         <v>1072</v>
@@ -17337,16 +17171,16 @@
     </row>
     <row r="73" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="2" t="s">
-        <v>665</v>
+        <v>1270</v>
       </c>
       <c r="B73" s="3" t="s">
         <v>666</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>1268</v>
+        <v>1271</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>1269</v>
+        <v>1272</v>
       </c>
       <c r="E73" s="2" t="s">
         <v>140</v>
@@ -17355,13 +17189,13 @@
         <v>1103</v>
       </c>
       <c r="G73" s="2" t="s">
-        <v>1138</v>
+        <v>1139</v>
       </c>
       <c r="H73" s="2" t="s">
         <v>1099</v>
       </c>
       <c r="I73" s="2" t="s">
-        <v>1140</v>
+        <v>1141</v>
       </c>
       <c r="K73" s="2" t="s">
         <v>116</v>
@@ -17373,7 +17207,7 @@
         <v>1073</v>
       </c>
       <c r="O73" s="2" t="s">
-        <v>1270</v>
+        <v>1273</v>
       </c>
       <c r="P73" s="2" t="s">
         <v>1116</v>
@@ -17394,7 +17228,7 @@
         <v>1</v>
       </c>
       <c r="Z73" s="2" t="s">
-        <v>1271</v>
+        <v>1274</v>
       </c>
       <c r="AA73" s="2" t="n">
         <v>5</v>
@@ -17408,7 +17242,7 @@
         <v>674</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>1272</v>
+        <v>1275</v>
       </c>
       <c r="D74" s="2" t="s">
         <v>1080</v>
@@ -17473,16 +17307,16 @@
         <v>680</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>1273</v>
+        <v>1276</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>1202</v>
+        <v>1204</v>
       </c>
       <c r="E75" s="2" t="s">
         <v>682</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>1240</v>
+        <v>1242</v>
       </c>
       <c r="G75" s="2" t="s">
         <v>1120</v>
@@ -17497,10 +17331,10 @@
         <v>1108</v>
       </c>
       <c r="O75" s="2" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="P75" s="2" t="s">
-        <v>1150</v>
+        <v>1151</v>
       </c>
       <c r="Q75" s="2" t="s">
         <v>1113</v>
@@ -17532,7 +17366,7 @@
         <v>687</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>1274</v>
+        <v>1277</v>
       </c>
       <c r="D76" s="2" t="s">
         <v>1068</v>
@@ -17541,7 +17375,7 @@
         <v>689</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>1148</v>
+        <v>1149</v>
       </c>
       <c r="G76" s="2" t="s">
         <v>1104</v>
@@ -17550,7 +17384,7 @@
         <v>1121</v>
       </c>
       <c r="I76" s="2" t="s">
-        <v>1166</v>
+        <v>1167</v>
       </c>
       <c r="K76" s="2" t="s">
         <v>282</v>
@@ -17568,7 +17402,7 @@
         <v>1074</v>
       </c>
       <c r="P76" s="2" t="s">
-        <v>1275</v>
+        <v>1278</v>
       </c>
       <c r="Q76" s="2" t="s">
         <v>1076</v>
@@ -17603,7 +17437,7 @@
         <v>697</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>1276</v>
+        <v>1279</v>
       </c>
       <c r="D77" s="2" t="s">
         <v>1068</v>
@@ -17668,7 +17502,7 @@
         <v>704</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>1277</v>
+        <v>1280</v>
       </c>
       <c r="D78" s="2" t="s">
         <v>1091</v>
@@ -17730,7 +17564,7 @@
         <v>710</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>1278</v>
+        <v>1281</v>
       </c>
       <c r="D79" s="2" t="s">
         <v>1068</v>
@@ -17739,7 +17573,7 @@
         <v>712</v>
       </c>
       <c r="F79" s="2" t="s">
-        <v>1279</v>
+        <v>1282</v>
       </c>
       <c r="G79" s="2" t="s">
         <v>1070</v>
@@ -17786,7 +17620,7 @@
         <v>717</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>1280</v>
+        <v>1283</v>
       </c>
       <c r="D80" s="2" t="s">
         <v>1096</v>
@@ -17804,7 +17638,7 @@
         <v>1099</v>
       </c>
       <c r="I80" s="2" t="s">
-        <v>1166</v>
+        <v>1167</v>
       </c>
       <c r="N80" s="2" t="s">
         <v>1073</v>
@@ -17813,7 +17647,7 @@
         <v>1074</v>
       </c>
       <c r="P80" s="2" t="s">
-        <v>1191</v>
+        <v>1193</v>
       </c>
       <c r="Q80" s="2" t="s">
         <v>1076</v>
@@ -17839,16 +17673,16 @@
     </row>
     <row r="81" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="2" t="s">
-        <v>722</v>
+        <v>1284</v>
       </c>
       <c r="B81" s="3" t="s">
         <v>723</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>1281</v>
+        <v>1285</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>1160</v>
+        <v>1161</v>
       </c>
       <c r="E81" s="2" t="s">
         <v>725</v>
@@ -17857,22 +17691,22 @@
         <v>1097</v>
       </c>
       <c r="G81" s="2" t="s">
-        <v>1203</v>
+        <v>1205</v>
       </c>
       <c r="H81" s="2" t="s">
-        <v>1161</v>
+        <v>1162</v>
       </c>
       <c r="I81" s="2" t="s">
-        <v>1140</v>
+        <v>1141</v>
       </c>
       <c r="N81" s="2" t="s">
         <v>1108</v>
       </c>
       <c r="O81" s="2" t="s">
-        <v>1162</v>
+        <v>1163</v>
       </c>
       <c r="P81" s="2" t="s">
-        <v>1135</v>
+        <v>1136</v>
       </c>
       <c r="Q81" s="2" t="s">
         <v>1113</v>
@@ -17901,7 +17735,7 @@
         <v>728</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>1282</v>
+        <v>1286</v>
       </c>
       <c r="D82" s="2" t="s">
         <v>1068</v>
@@ -17910,7 +17744,7 @@
         <v>730</v>
       </c>
       <c r="F82" s="2" t="s">
-        <v>1283</v>
+        <v>1287</v>
       </c>
       <c r="G82" s="2" t="s">
         <v>1120</v>
@@ -17919,7 +17753,7 @@
         <v>1071</v>
       </c>
       <c r="I82" s="2" t="s">
-        <v>1140</v>
+        <v>1141</v>
       </c>
       <c r="L82" s="2" t="s">
         <v>732</v>
@@ -17960,7 +17794,7 @@
         <v>736</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>1284</v>
+        <v>1288</v>
       </c>
       <c r="D83" s="2" t="s">
         <v>1068</v>
@@ -17969,7 +17803,7 @@
         <v>313</v>
       </c>
       <c r="F83" s="2" t="s">
-        <v>1173</v>
+        <v>1175</v>
       </c>
       <c r="G83" s="2" t="s">
         <v>1070</v>
@@ -17990,7 +17824,7 @@
         <v>1074</v>
       </c>
       <c r="P83" s="2" t="s">
-        <v>1150</v>
+        <v>1151</v>
       </c>
       <c r="Q83" s="2" t="s">
         <v>1076</v>
@@ -18025,7 +17859,7 @@
         <v>742</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>1285</v>
+        <v>1289</v>
       </c>
       <c r="D84" s="2" t="s">
         <v>1096</v>
@@ -18037,10 +17871,10 @@
         <v>1092</v>
       </c>
       <c r="G84" s="2" t="s">
-        <v>1138</v>
+        <v>1139</v>
       </c>
       <c r="H84" s="2" t="s">
-        <v>1245</v>
+        <v>1247</v>
       </c>
       <c r="I84" s="2" t="s">
         <v>1126</v>
@@ -18049,7 +17883,7 @@
         <v>745</v>
       </c>
       <c r="N84" s="2" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="O84" s="2" t="s">
         <v>1074</v>
@@ -18090,19 +17924,19 @@
         <v>751</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>1286</v>
+        <v>1290</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>1217</v>
+        <v>1218</v>
       </c>
       <c r="E85" s="2" t="s">
         <v>753</v>
       </c>
       <c r="F85" s="2" t="s">
-        <v>1235</v>
+        <v>1237</v>
       </c>
       <c r="G85" s="2" t="s">
-        <v>1145</v>
+        <v>1146</v>
       </c>
       <c r="H85" s="2" t="s">
         <v>1121</v>
@@ -18114,7 +17948,7 @@
         <v>1108</v>
       </c>
       <c r="O85" s="2" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="P85" s="2" t="s">
         <v>1105</v>
@@ -18149,7 +17983,7 @@
         <v>757</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>1287</v>
+        <v>1291</v>
       </c>
       <c r="D86" s="2" t="s">
         <v>1068</v>
@@ -18208,7 +18042,7 @@
         <v>763</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>1288</v>
+        <v>1292</v>
       </c>
       <c r="D87" s="2" t="s">
         <v>1068</v>
@@ -18220,13 +18054,13 @@
         <v>1103</v>
       </c>
       <c r="G87" s="2" t="s">
-        <v>1138</v>
+        <v>1139</v>
       </c>
       <c r="H87" s="2" t="s">
         <v>1099</v>
       </c>
       <c r="I87" s="2" t="s">
-        <v>1140</v>
+        <v>1141</v>
       </c>
       <c r="K87" s="2" t="s">
         <v>116</v>
@@ -18235,10 +18069,10 @@
         <v>1108</v>
       </c>
       <c r="O87" s="2" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="P87" s="2" t="s">
-        <v>1135</v>
+        <v>1136</v>
       </c>
       <c r="Q87" s="2" t="s">
         <v>765</v>
@@ -18270,7 +18104,7 @@
         <v>767</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>1289</v>
+        <v>1293</v>
       </c>
       <c r="D88" s="2" t="s">
         <v>1096</v>
@@ -18312,7 +18146,7 @@
         <v>770</v>
       </c>
       <c r="T88" s="2" t="s">
-        <v>1290</v>
+        <v>1294</v>
       </c>
       <c r="V88" s="2" t="s">
         <v>772</v>
@@ -18341,7 +18175,7 @@
         <v>776</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>1291</v>
+        <v>1295</v>
       </c>
       <c r="D89" s="2" t="s">
         <v>1080</v>
@@ -18350,7 +18184,7 @@
         <v>778</v>
       </c>
       <c r="F89" s="2" t="s">
-        <v>1148</v>
+        <v>1149</v>
       </c>
       <c r="G89" s="2" t="s">
         <v>1070</v>
@@ -18362,7 +18196,7 @@
         <v>1126</v>
       </c>
       <c r="J89" s="2" t="s">
-        <v>1292</v>
+        <v>1296</v>
       </c>
       <c r="K89" s="2" t="s">
         <v>205</v>
@@ -18383,7 +18217,7 @@
         <v>165</v>
       </c>
       <c r="T89" s="2" t="s">
-        <v>1293</v>
+        <v>1297</v>
       </c>
       <c r="V89" s="2" t="s">
         <v>781</v>
@@ -18409,7 +18243,7 @@
         <v>784</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>1294</v>
+        <v>1298</v>
       </c>
       <c r="D90" s="2" t="s">
         <v>1096</v>
@@ -18451,7 +18285,7 @@
         <v>1077</v>
       </c>
       <c r="T90" s="2" t="s">
-        <v>1295</v>
+        <v>1299</v>
       </c>
       <c r="W90" s="2" t="s">
         <v>519</v>
@@ -18477,7 +18311,7 @@
         <v>792</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>1296</v>
+        <v>1300</v>
       </c>
       <c r="D91" s="2" t="s">
         <v>1080</v>
@@ -18489,7 +18323,7 @@
         <v>576</v>
       </c>
       <c r="G91" s="2" t="s">
-        <v>1145</v>
+        <v>1146</v>
       </c>
       <c r="H91" s="2" t="s">
         <v>1083</v>
@@ -18522,7 +18356,7 @@
         <v>795</v>
       </c>
       <c r="T91" s="2" t="s">
-        <v>1297</v>
+        <v>1301</v>
       </c>
       <c r="V91" s="2" t="s">
         <v>797</v>
@@ -18548,7 +18382,7 @@
         <v>800</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>1298</v>
+        <v>1302</v>
       </c>
       <c r="D92" s="2" t="s">
         <v>1091</v>
@@ -18575,7 +18409,7 @@
         <v>1074</v>
       </c>
       <c r="P92" s="2" t="s">
-        <v>1191</v>
+        <v>1193</v>
       </c>
       <c r="Q92" s="2" t="s">
         <v>803</v>
@@ -18604,7 +18438,7 @@
         <v>806</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>1299</v>
+        <v>1303</v>
       </c>
       <c r="D93" s="2" t="s">
         <v>1096</v>
@@ -18634,7 +18468,7 @@
         <v>1074</v>
       </c>
       <c r="P93" s="2" t="s">
-        <v>1150</v>
+        <v>1151</v>
       </c>
       <c r="Q93" s="2" t="s">
         <v>1076</v>
@@ -18661,7 +18495,7 @@
         <v>5</v>
       </c>
       <c r="AD93" s="2" t="s">
-        <v>1300</v>
+        <v>1304</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18672,7 +18506,7 @@
         <v>813</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>1301</v>
+        <v>1305</v>
       </c>
       <c r="D94" s="2" t="s">
         <v>1068</v>
@@ -18696,7 +18530,7 @@
         <v>1108</v>
       </c>
       <c r="O94" s="2" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="P94" s="2" t="s">
         <v>1116</v>
@@ -18705,7 +18539,7 @@
         <v>1113</v>
       </c>
       <c r="R94" s="2" t="s">
-        <v>1187</v>
+        <v>1189</v>
       </c>
       <c r="X94" s="2" t="n">
         <v>1</v>
@@ -18725,10 +18559,10 @@
         <v>817</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>1302</v>
+        <v>1306</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>1160</v>
+        <v>1161</v>
       </c>
       <c r="E95" s="2" t="s">
         <v>819</v>
@@ -18740,13 +18574,13 @@
         <v>1115</v>
       </c>
       <c r="I95" s="2" t="s">
-        <v>1140</v>
+        <v>1141</v>
       </c>
       <c r="N95" s="2" t="s">
         <v>273</v>
       </c>
       <c r="O95" s="2" t="s">
-        <v>1162</v>
+        <v>1163</v>
       </c>
       <c r="Q95" s="2" t="s">
         <v>1113</v>
@@ -18775,7 +18609,7 @@
         <v>823</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>1303</v>
+        <v>1307</v>
       </c>
       <c r="D96" s="2" t="s">
         <v>1096</v>
@@ -18805,7 +18639,7 @@
         <v>1074</v>
       </c>
       <c r="P96" s="2" t="s">
-        <v>1150</v>
+        <v>1151</v>
       </c>
       <c r="Q96" s="2" t="s">
         <v>1113</v>
@@ -18834,16 +18668,16 @@
         <v>828</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>1304</v>
+        <v>1308</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>1202</v>
+        <v>1204</v>
       </c>
       <c r="E97" s="2" t="s">
         <v>830</v>
       </c>
       <c r="F97" s="2" t="s">
-        <v>1305</v>
+        <v>1309</v>
       </c>
       <c r="G97" s="2" t="s">
         <v>1104</v>
@@ -18861,7 +18695,7 @@
         <v>1074</v>
       </c>
       <c r="P97" s="2" t="s">
-        <v>1150</v>
+        <v>1151</v>
       </c>
       <c r="Q97" s="2" t="s">
         <v>832</v>
@@ -18893,7 +18727,7 @@
         <v>835</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>1306</v>
+        <v>1310</v>
       </c>
       <c r="D98" s="2" t="s">
         <v>1068</v>
@@ -18958,7 +18792,7 @@
         <v>842</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>1307</v>
+        <v>1311</v>
       </c>
       <c r="D99" s="2" t="s">
         <v>1096</v>
@@ -18967,7 +18801,7 @@
         <v>844</v>
       </c>
       <c r="F99" s="2" t="s">
-        <v>1235</v>
+        <v>1237</v>
       </c>
       <c r="G99" s="2" t="s">
         <v>1070</v>
@@ -19006,7 +18840,7 @@
         <v>847</v>
       </c>
       <c r="T99" s="2" t="s">
-        <v>1308</v>
+        <v>1312</v>
       </c>
       <c r="W99" s="2" t="s">
         <v>849</v>
@@ -19032,10 +18866,10 @@
         <v>852</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>1309</v>
+        <v>1313</v>
       </c>
       <c r="D100" s="2" t="s">
-        <v>1160</v>
+        <v>1161</v>
       </c>
       <c r="E100" s="2" t="s">
         <v>854</v>
@@ -19074,7 +18908,7 @@
         <v>1077</v>
       </c>
       <c r="U100" s="2" t="s">
-        <v>1310</v>
+        <v>1314</v>
       </c>
       <c r="W100" s="2" t="s">
         <v>570</v>
@@ -19089,7 +18923,7 @@
         <v>858</v>
       </c>
     </row>
-    <row r="101" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="101" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="2" t="s">
         <v>859</v>
       </c>
@@ -19097,10 +18931,10 @@
         <v>860</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>1311</v>
+        <v>1315</v>
       </c>
       <c r="D101" s="2" t="s">
-        <v>1134</v>
+        <v>1135</v>
       </c>
       <c r="E101" s="2" t="s">
         <v>862</v>
@@ -19118,7 +18952,7 @@
         <v>1126</v>
       </c>
       <c r="J101" s="2" t="s">
-        <v>1181</v>
+        <v>1183</v>
       </c>
       <c r="K101" s="2" t="s">
         <v>116</v>
@@ -19142,7 +18976,7 @@
         <v>118</v>
       </c>
       <c r="T101" s="2" t="s">
-        <v>1312</v>
+        <v>1316</v>
       </c>
       <c r="X101" s="2" t="n">
         <v>1</v>
@@ -19165,7 +18999,7 @@
         <v>867</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>1313</v>
+        <v>1317</v>
       </c>
       <c r="D102" s="2" t="s">
         <v>1091</v>
@@ -19177,22 +19011,22 @@
         <v>1097</v>
       </c>
       <c r="G102" s="2" t="s">
-        <v>1263</v>
+        <v>1265</v>
       </c>
       <c r="H102" s="2" t="s">
-        <v>1161</v>
+        <v>1162</v>
       </c>
       <c r="I102" s="2" t="s">
         <v>1072</v>
       </c>
       <c r="J102" s="2" t="s">
-        <v>1314</v>
+        <v>1318</v>
       </c>
       <c r="N102" s="2" t="s">
         <v>1073</v>
       </c>
       <c r="O102" s="2" t="s">
-        <v>1162</v>
+        <v>1163</v>
       </c>
       <c r="Q102" s="2" t="s">
         <v>1076</v>
@@ -19221,7 +19055,7 @@
         <v>872</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>1315</v>
+        <v>1319</v>
       </c>
       <c r="D103" s="2" t="s">
         <v>1080</v>
@@ -19239,7 +19073,7 @@
         <v>1099</v>
       </c>
       <c r="I103" s="2" t="s">
-        <v>1166</v>
+        <v>1167</v>
       </c>
       <c r="K103" s="2" t="s">
         <v>116</v>
@@ -19254,13 +19088,13 @@
         <v>1074</v>
       </c>
       <c r="P103" s="2" t="s">
-        <v>1150</v>
+        <v>1151</v>
       </c>
       <c r="Q103" s="2" t="s">
         <v>1076</v>
       </c>
       <c r="R103" s="2" t="s">
-        <v>1316</v>
+        <v>1320</v>
       </c>
       <c r="X103" s="2" t="n">
         <v>1</v>
@@ -19283,7 +19117,7 @@
         <v>879</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>1317</v>
+        <v>1321</v>
       </c>
       <c r="D104" s="2" t="s">
         <v>1080</v>
@@ -19298,7 +19132,7 @@
         <v>1070</v>
       </c>
       <c r="H104" s="2" t="s">
-        <v>1156</v>
+        <v>1157</v>
       </c>
       <c r="I104" s="2" t="s">
         <v>1084</v>
@@ -19313,7 +19147,7 @@
         <v>1086</v>
       </c>
       <c r="O104" s="2" t="s">
-        <v>1146</v>
+        <v>1147</v>
       </c>
       <c r="P104" s="2" t="s">
         <v>1087</v>
@@ -19351,7 +19185,7 @@
         <v>886</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>1318</v>
+        <v>1322</v>
       </c>
       <c r="D105" s="2" t="s">
         <v>1096</v>
@@ -19360,7 +19194,7 @@
         <v>888</v>
       </c>
       <c r="F105" s="2" t="s">
-        <v>1319</v>
+        <v>1323</v>
       </c>
       <c r="G105" s="2" t="s">
         <v>1082</v>
@@ -19413,7 +19247,7 @@
         <v>893</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>1320</v>
+        <v>1324</v>
       </c>
       <c r="D106" s="2" t="s">
         <v>1096</v>
@@ -19422,7 +19256,7 @@
         <v>895</v>
       </c>
       <c r="F106" s="2" t="s">
-        <v>1321</v>
+        <v>1325</v>
       </c>
       <c r="G106" s="2" t="s">
         <v>1082</v>
@@ -19434,7 +19268,7 @@
         <v>1126</v>
       </c>
       <c r="K106" s="2" t="s">
-        <v>1322</v>
+        <v>1326</v>
       </c>
       <c r="N106" s="2" t="s">
         <v>1100</v>
@@ -19475,7 +19309,7 @@
         <v>901</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>1323</v>
+        <v>1327</v>
       </c>
       <c r="D107" s="2" t="s">
         <v>1096</v>
@@ -19505,7 +19339,7 @@
         <v>1074</v>
       </c>
       <c r="P107" s="2" t="s">
-        <v>1191</v>
+        <v>1193</v>
       </c>
       <c r="Q107" s="2" t="s">
         <v>904</v>
@@ -19514,7 +19348,7 @@
         <v>76</v>
       </c>
       <c r="U107" s="2" t="s">
-        <v>1324</v>
+        <v>1328</v>
       </c>
       <c r="V107" s="2" t="s">
         <v>906</v>
@@ -19543,7 +19377,7 @@
         <v>908</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>1325</v>
+        <v>1329</v>
       </c>
       <c r="D108" s="2" t="s">
         <v>1096</v>
@@ -19552,16 +19386,16 @@
         <v>910</v>
       </c>
       <c r="F108" s="2" t="s">
-        <v>1326</v>
+        <v>1330</v>
       </c>
       <c r="G108" s="2" t="s">
-        <v>1145</v>
+        <v>1146</v>
       </c>
       <c r="H108" s="2" t="s">
-        <v>1327</v>
+        <v>1331</v>
       </c>
       <c r="I108" s="2" t="s">
-        <v>1328</v>
+        <v>1332</v>
       </c>
       <c r="K108" s="2" t="s">
         <v>116</v>
@@ -19576,7 +19410,7 @@
         <v>1100</v>
       </c>
       <c r="O108" s="2" t="s">
-        <v>1329</v>
+        <v>1333</v>
       </c>
       <c r="P108" s="2" t="s">
         <v>1087</v>
@@ -19617,7 +19451,7 @@
         <v>921</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>1330</v>
+        <v>1334</v>
       </c>
       <c r="D109" s="2" t="s">
         <v>1068</v>
@@ -19626,13 +19460,13 @@
         <v>923</v>
       </c>
       <c r="F109" s="2" t="s">
-        <v>1240</v>
+        <v>1242</v>
       </c>
       <c r="G109" s="2" t="s">
         <v>1120</v>
       </c>
       <c r="H109" s="2" t="s">
-        <v>1156</v>
+        <v>1157</v>
       </c>
       <c r="I109" s="2" t="s">
         <v>1072</v>
@@ -19665,7 +19499,7 @@
         <v>927</v>
       </c>
       <c r="T109" s="2" t="s">
-        <v>1308</v>
+        <v>1312</v>
       </c>
       <c r="W109" s="2" t="s">
         <v>928</v>
@@ -19691,7 +19525,7 @@
         <v>932</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>1182</v>
+        <v>1184</v>
       </c>
       <c r="D110" s="2" t="s">
         <v>1068</v>
@@ -19712,7 +19546,7 @@
         <v>1081</v>
       </c>
       <c r="J110" s="2" t="s">
-        <v>1331</v>
+        <v>1335</v>
       </c>
       <c r="N110" s="2" t="s">
         <v>1073</v>
@@ -19747,10 +19581,10 @@
         <v>937</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>1332</v>
+        <v>1336</v>
       </c>
       <c r="D111" s="2" t="s">
-        <v>1160</v>
+        <v>1161</v>
       </c>
       <c r="E111" s="2" t="s">
         <v>271</v>
@@ -19759,19 +19593,19 @@
         <v>1104</v>
       </c>
       <c r="G111" s="2" t="s">
-        <v>1203</v>
+        <v>1205</v>
       </c>
       <c r="H111" s="2" t="s">
-        <v>1161</v>
+        <v>1162</v>
       </c>
       <c r="I111" s="2" t="s">
-        <v>1140</v>
+        <v>1141</v>
       </c>
       <c r="N111" s="2" t="s">
         <v>273</v>
       </c>
       <c r="O111" s="2" t="s">
-        <v>1162</v>
+        <v>1163</v>
       </c>
       <c r="Q111" s="2" t="s">
         <v>1113</v>
@@ -19800,7 +19634,7 @@
         <v>940</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>1333</v>
+        <v>1337</v>
       </c>
       <c r="D112" s="2" t="s">
         <v>1068</v>
@@ -19809,7 +19643,7 @@
         <v>942</v>
       </c>
       <c r="F112" s="2" t="s">
-        <v>1148</v>
+        <v>1149</v>
       </c>
       <c r="G112" s="2" t="s">
         <v>1104</v>
@@ -19836,7 +19670,7 @@
         <v>1074</v>
       </c>
       <c r="P112" s="2" t="s">
-        <v>1275</v>
+        <v>1278</v>
       </c>
       <c r="Q112" s="2" t="s">
         <v>1076</v>
@@ -19874,7 +19708,7 @@
         <v>948</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>1334</v>
+        <v>1338</v>
       </c>
       <c r="D113" s="2" t="s">
         <v>1096</v>
@@ -19942,10 +19776,10 @@
         <v>958</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>1335</v>
+        <v>1339</v>
       </c>
       <c r="D114" s="2" t="s">
-        <v>1134</v>
+        <v>1135</v>
       </c>
       <c r="E114" s="2" t="s">
         <v>960</v>
@@ -19963,7 +19797,7 @@
         <v>1108</v>
       </c>
       <c r="O114" s="2" t="s">
-        <v>1270</v>
+        <v>1273</v>
       </c>
       <c r="P114" s="2" t="s">
         <v>1116</v>
@@ -19972,7 +19806,7 @@
         <v>1113</v>
       </c>
       <c r="R114" s="2" t="s">
-        <v>1187</v>
+        <v>1189</v>
       </c>
       <c r="X114" s="2" t="n">
         <v>0</v>
@@ -19981,7 +19815,7 @@
         <v>1</v>
       </c>
       <c r="Z114" s="2" t="s">
-        <v>1336</v>
+        <v>1340</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19992,7 +19826,7 @@
         <v>963</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>1337</v>
+        <v>1341</v>
       </c>
       <c r="D115" s="2" t="s">
         <v>1091</v>
@@ -20004,19 +19838,19 @@
         <v>1104</v>
       </c>
       <c r="G115" s="2" t="s">
-        <v>1203</v>
+        <v>1205</v>
       </c>
       <c r="H115" s="2" t="s">
-        <v>1161</v>
+        <v>1162</v>
       </c>
       <c r="I115" s="2" t="s">
-        <v>1140</v>
+        <v>1141</v>
       </c>
       <c r="N115" s="2" t="s">
         <v>1108</v>
       </c>
       <c r="O115" s="2" t="s">
-        <v>1162</v>
+        <v>1163</v>
       </c>
       <c r="Q115" s="2" t="s">
         <v>1113</v>
@@ -20045,7 +19879,7 @@
         <v>967</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>1338</v>
+        <v>1342</v>
       </c>
       <c r="D116" s="2" t="s">
         <v>1096</v>
@@ -20081,7 +19915,7 @@
         <v>1077</v>
       </c>
       <c r="U116" s="2" t="s">
-        <v>1339</v>
+        <v>1343</v>
       </c>
       <c r="V116" s="2" t="s">
         <v>971</v>
@@ -20110,10 +19944,10 @@
         <v>975</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>1340</v>
+        <v>1344</v>
       </c>
       <c r="D117" s="2" t="s">
-        <v>1202</v>
+        <v>1204</v>
       </c>
       <c r="E117" s="2" t="s">
         <v>977</v>
@@ -20128,7 +19962,7 @@
         <v>1099</v>
       </c>
       <c r="I117" s="2" t="s">
-        <v>1140</v>
+        <v>1141</v>
       </c>
       <c r="N117" s="2" t="s">
         <v>1108</v>
@@ -20137,7 +19971,7 @@
         <v>1074</v>
       </c>
       <c r="P117" s="2" t="s">
-        <v>1150</v>
+        <v>1151</v>
       </c>
       <c r="Q117" s="2" t="s">
         <v>1113</v>
@@ -20166,7 +20000,7 @@
         <v>980</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>1341</v>
+        <v>1345</v>
       </c>
       <c r="D118" s="2" t="s">
         <v>1068</v>
@@ -20190,13 +20024,13 @@
         <v>1074</v>
       </c>
       <c r="P118" s="2" t="s">
-        <v>1135</v>
+        <v>1136</v>
       </c>
       <c r="Q118" s="2" t="s">
         <v>1113</v>
       </c>
       <c r="R118" s="2" t="s">
-        <v>1187</v>
+        <v>1189</v>
       </c>
       <c r="X118" s="2" t="n">
         <v>1</v>
@@ -20213,7 +20047,7 @@
         <v>984</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>1342</v>
+        <v>1346</v>
       </c>
       <c r="D119" s="2" t="s">
         <v>1068</v>
@@ -20222,7 +20056,7 @@
         <v>730</v>
       </c>
       <c r="F119" s="2" t="s">
-        <v>1343</v>
+        <v>1347</v>
       </c>
       <c r="G119" s="2" t="s">
         <v>1120</v>
@@ -20240,30 +20074,30 @@
         <v>1108</v>
       </c>
       <c r="O119" s="2" t="s">
-        <v>1146</v>
+        <v>1147</v>
       </c>
       <c r="P119" s="2" t="s">
-        <v>1135</v>
+        <v>1136</v>
       </c>
       <c r="Q119" s="2" t="s">
         <v>1113</v>
       </c>
       <c r="R119" s="2" t="s">
-        <v>1187</v>
+        <v>1189</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="2" t="s">
-        <v>988</v>
+        <v>1348</v>
       </c>
       <c r="B120" s="3" t="s">
         <v>989</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>1344</v>
+        <v>1349</v>
       </c>
       <c r="D120" s="2" t="s">
-        <v>1160</v>
+        <v>1161</v>
       </c>
       <c r="E120" s="2" t="s">
         <v>725</v>
@@ -20275,16 +20109,16 @@
         <v>1104</v>
       </c>
       <c r="H120" s="2" t="s">
-        <v>1161</v>
+        <v>1162</v>
       </c>
       <c r="I120" s="2" t="s">
-        <v>1140</v>
+        <v>1141</v>
       </c>
       <c r="N120" s="2" t="s">
         <v>1073</v>
       </c>
       <c r="O120" s="2" t="s">
-        <v>1162</v>
+        <v>1163</v>
       </c>
       <c r="P120" s="2" t="s">
         <v>1087</v>
@@ -20316,7 +20150,7 @@
         <v>993</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>1345</v>
+        <v>1350</v>
       </c>
       <c r="D121" s="2" t="s">
         <v>1096</v>
@@ -20346,7 +20180,7 @@
         <v>1074</v>
       </c>
       <c r="P121" s="2" t="s">
-        <v>1179</v>
+        <v>1181</v>
       </c>
       <c r="Q121" s="2" t="s">
         <v>1076</v>
@@ -20381,7 +20215,7 @@
         <v>1001</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>1346</v>
+        <v>1351</v>
       </c>
       <c r="D122" s="2" t="s">
         <v>1080</v>
@@ -20390,13 +20224,13 @@
         <v>1000</v>
       </c>
       <c r="F122" s="2" t="s">
-        <v>1235</v>
+        <v>1237</v>
       </c>
       <c r="G122" s="2" t="s">
         <v>1070</v>
       </c>
       <c r="H122" s="2" t="s">
-        <v>1156</v>
+        <v>1157</v>
       </c>
       <c r="I122" s="2" t="s">
         <v>1072</v>
@@ -20429,7 +20263,7 @@
         <v>439</v>
       </c>
       <c r="T122" s="2" t="s">
-        <v>1347</v>
+        <v>1352</v>
       </c>
       <c r="W122" s="2" t="s">
         <v>1007</v>
@@ -20455,7 +20289,7 @@
         <v>1010</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>1348</v>
+        <v>1353</v>
       </c>
       <c r="D123" s="2" t="s">
         <v>1068</v>
@@ -20476,16 +20310,16 @@
         <v>1086</v>
       </c>
       <c r="O123" s="2" t="s">
-        <v>1146</v>
+        <v>1147</v>
       </c>
       <c r="P123" s="2" t="s">
-        <v>1186</v>
+        <v>1188</v>
       </c>
       <c r="Q123" s="2" t="s">
         <v>1113</v>
       </c>
       <c r="R123" s="2" t="s">
-        <v>1187</v>
+        <v>1189</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20496,7 +20330,7 @@
         <v>1014</v>
       </c>
       <c r="C124" s="2" t="s">
-        <v>1349</v>
+        <v>1354</v>
       </c>
       <c r="D124" s="2" t="s">
         <v>1080</v>
@@ -20508,13 +20342,13 @@
         <v>1131</v>
       </c>
       <c r="G124" s="2" t="s">
-        <v>1145</v>
+        <v>1146</v>
       </c>
       <c r="H124" s="2" t="s">
-        <v>1156</v>
+        <v>1157</v>
       </c>
       <c r="I124" s="2" t="s">
-        <v>1350</v>
+        <v>1355</v>
       </c>
       <c r="K124" s="2" t="s">
         <v>1018</v>
@@ -20523,10 +20357,10 @@
         <v>1019</v>
       </c>
       <c r="N124" s="2" t="s">
-        <v>1351</v>
+        <v>1356</v>
       </c>
       <c r="O124" s="2" t="s">
-        <v>1146</v>
+        <v>1147</v>
       </c>
       <c r="P124" s="2" t="s">
         <v>1105</v>
@@ -20567,7 +20401,7 @@
         <v>1025</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>1352</v>
+        <v>1357</v>
       </c>
       <c r="D125" s="2" t="s">
         <v>1068</v>
@@ -20576,25 +20410,25 @@
         <v>1027</v>
       </c>
       <c r="F125" s="2" t="s">
-        <v>1321</v>
+        <v>1325</v>
       </c>
       <c r="G125" s="2" t="s">
         <v>1120</v>
       </c>
       <c r="H125" s="2" t="s">
-        <v>1253</v>
+        <v>1255</v>
       </c>
       <c r="I125" s="2" t="s">
-        <v>1140</v>
+        <v>1141</v>
       </c>
       <c r="N125" s="2" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="O125" s="2" t="s">
-        <v>1270</v>
+        <v>1273</v>
       </c>
       <c r="P125" s="2" t="s">
-        <v>1275</v>
+        <v>1278</v>
       </c>
       <c r="Q125" s="2" t="s">
         <v>1113</v>
@@ -20620,7 +20454,7 @@
         <v>1030</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>1353</v>
+        <v>1358</v>
       </c>
       <c r="D126" s="2" t="s">
         <v>1080</v>
@@ -20635,7 +20469,7 @@
         <v>1115</v>
       </c>
       <c r="H126" s="2" t="s">
-        <v>1354</v>
+        <v>1359</v>
       </c>
       <c r="I126" s="2" t="s">
         <v>1072</v>
@@ -20656,13 +20490,13 @@
         <v>1087</v>
       </c>
       <c r="Q126" s="2" t="s">
-        <v>1355</v>
+        <v>1360</v>
       </c>
       <c r="R126" s="2" t="s">
         <v>275</v>
       </c>
       <c r="S126" s="2" t="s">
-        <v>1356</v>
+        <v>1361</v>
       </c>
       <c r="V126" s="2" t="s">
         <v>1037</v>
@@ -20688,7 +20522,7 @@
         <v>1040</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>1357</v>
+        <v>1362</v>
       </c>
       <c r="D127" s="2" t="s">
         <v>1096</v>
@@ -20715,7 +20549,7 @@
         <v>1074</v>
       </c>
       <c r="P127" s="2" t="s">
-        <v>1179</v>
+        <v>1181</v>
       </c>
       <c r="Q127" s="2" t="s">
         <v>567</v>
@@ -20724,7 +20558,7 @@
         <v>1077</v>
       </c>
       <c r="T127" s="2" t="s">
-        <v>1243</v>
+        <v>1245</v>
       </c>
       <c r="V127" s="2" t="s">
         <v>563</v>
@@ -20744,13 +20578,13 @@
     </row>
     <row r="128" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="2" t="s">
-        <v>1043</v>
+        <v>1363</v>
       </c>
       <c r="B128" s="3" t="s">
         <v>1044</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>1358</v>
+        <v>1364</v>
       </c>
       <c r="D128" s="2" t="s">
         <v>1068</v>
@@ -20786,7 +20620,7 @@
         <v>1110</v>
       </c>
       <c r="T128" s="2" t="s">
-        <v>1359</v>
+        <v>1365</v>
       </c>
       <c r="W128" s="2" t="s">
         <v>327</v>
@@ -20806,19 +20640,19 @@
         <v>1049</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>1360</v>
+        <v>1366</v>
       </c>
       <c r="E129" s="2" t="s">
         <v>1051</v>
       </c>
       <c r="N129" s="2" t="s">
-        <v>1361</v>
+        <v>1367</v>
       </c>
       <c r="Q129" s="2" t="s">
-        <v>1362</v>
+        <v>1368</v>
       </c>
       <c r="S129" s="2" t="s">
-        <v>1363</v>
+        <v>1369</v>
       </c>
       <c r="U129" s="3" t="s">
         <v>1054</v>
@@ -20832,19 +20666,19 @@
         <v>1056</v>
       </c>
       <c r="C130" s="2" t="s">
-        <v>1364</v>
+        <v>1370</v>
       </c>
       <c r="E130" s="2" t="s">
-        <v>1365</v>
+        <v>1371</v>
       </c>
       <c r="N130" s="2" t="s">
-        <v>1361</v>
+        <v>1367</v>
       </c>
       <c r="Q130" s="2" t="s">
-        <v>1366</v>
+        <v>1372</v>
       </c>
       <c r="S130" s="2" t="s">
-        <v>1363</v>
+        <v>1369</v>
       </c>
       <c r="U130" s="3" t="s">
         <v>1059</v>
@@ -20861,19 +20695,19 @@
         <v>1062</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>1367</v>
+        <v>1373</v>
       </c>
       <c r="E131" s="2" t="s">
         <v>1064</v>
       </c>
       <c r="N131" s="2" t="s">
-        <v>1361</v>
+        <v>1367</v>
       </c>
       <c r="Q131" s="2" t="s">
         <v>1076</v>
       </c>
       <c r="S131" s="2" t="s">
-        <v>1368</v>
+        <v>1374</v>
       </c>
       <c r="U131" s="3" t="s">
         <v>1066</v>

</xml_diff>